<commit_message>
Add data for 2023-07-07
</commit_message>
<xml_diff>
--- a/output/index-crime-ytd.xlsx
+++ b/output/index-crime-ytd.xlsx
@@ -62,8 +62,8 @@
     <sheet name="Chicago Lawn" sheetId="53" r:id="rId53"/>
     <sheet name="Sheffield &amp; DePaul" sheetId="54" r:id="rId54"/>
     <sheet name="Washington Park" sheetId="55" r:id="rId55"/>
-    <sheet name="Douglas" sheetId="56" r:id="rId56"/>
-    <sheet name="Grand Crossing" sheetId="57" r:id="rId57"/>
+    <sheet name="Grand Crossing" sheetId="56" r:id="rId56"/>
+    <sheet name="Douglas" sheetId="57" r:id="rId57"/>
     <sheet name="Dunning" sheetId="58" r:id="rId58"/>
     <sheet name="Avalon Park" sheetId="59" r:id="rId59"/>
     <sheet name="Boystown" sheetId="60" r:id="rId60"/>
@@ -102,9 +102,9 @@
     <sheet name="Sauganash,Forest Glen" sheetId="93" r:id="rId93"/>
     <sheet name="Rush &amp; Division" sheetId="94" r:id="rId94"/>
     <sheet name="Burnside" sheetId="95" r:id="rId95"/>
-    <sheet name="Grant Park" sheetId="96" r:id="rId96"/>
+    <sheet name="Printers Row" sheetId="96" r:id="rId96"/>
     <sheet name="Gold Coast" sheetId="97" r:id="rId97"/>
-    <sheet name="Printers Row" sheetId="98" r:id="rId98"/>
+    <sheet name="Grant Park" sheetId="98" r:id="rId98"/>
     <sheet name="Museum Campus" sheetId="99" r:id="rId99"/>
     <sheet name="Millenium Park" sheetId="100" r:id="rId100"/>
   </sheets>
@@ -20830,28 +20830,28 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="E2">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="F2">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="G2">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="I2">
-        <v>31</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -20859,28 +20859,31 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="D3">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="F3">
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="G3">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="H3">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="I3">
-        <v>40</v>
+        <v>118</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -20888,12 +20891,27 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
@@ -20902,28 +20920,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>26</v>
+        <v>162</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>169</v>
       </c>
       <c r="D5">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="E5">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F5">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="I5">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -20931,28 +20949,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I6">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -20960,31 +20978,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -20992,28 +21010,28 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="C8">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D8">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="E8">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="F8">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="G8">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="H8">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="I8">
-        <v>121</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21021,28 +21039,28 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="C9">
-        <v>67</v>
+        <v>179</v>
       </c>
       <c r="D9">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="E9">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="F9">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="G9">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="H9">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="I9">
-        <v>35</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21050,28 +21068,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>270</v>
+        <v>478</v>
       </c>
       <c r="C10">
-        <v>365</v>
+        <v>529</v>
       </c>
       <c r="D10">
-        <v>374</v>
+        <v>455</v>
       </c>
       <c r="E10">
-        <v>354</v>
+        <v>496</v>
       </c>
       <c r="F10">
-        <v>344</v>
+        <v>432</v>
       </c>
       <c r="G10">
-        <v>236</v>
+        <v>376</v>
       </c>
       <c r="H10">
-        <v>240</v>
+        <v>325</v>
       </c>
       <c r="I10">
-        <v>319</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21079,31 +21097,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>447</v>
+        <v>1101</v>
       </c>
       <c r="C11">
-        <v>564</v>
+        <v>1261</v>
       </c>
       <c r="D11">
-        <v>577</v>
+        <v>1201</v>
       </c>
       <c r="E11">
-        <v>570</v>
+        <v>1159</v>
       </c>
       <c r="F11">
-        <v>531</v>
+        <v>1120</v>
       </c>
       <c r="G11">
-        <v>422</v>
+        <v>1064</v>
       </c>
       <c r="H11">
-        <v>454</v>
+        <v>1027</v>
       </c>
       <c r="I11">
-        <v>581</v>
+        <v>1103</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -21168,28 +21186,28 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E2">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="F2">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="G2">
-        <v>127</v>
+        <v>26</v>
       </c>
       <c r="H2">
-        <v>138</v>
+        <v>30</v>
       </c>
       <c r="I2">
-        <v>126</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -21197,31 +21215,28 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>125</v>
+        <v>34</v>
       </c>
       <c r="C3">
-        <v>149</v>
+        <v>35</v>
       </c>
       <c r="D3">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="E3">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="F3">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="G3">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="H3">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="I3">
-        <v>118</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -21229,27 +21244,12 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
     </row>
@@ -21258,28 +21258,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>148</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <v>141</v>
+        <v>24</v>
       </c>
       <c r="F5">
-        <v>140</v>
+        <v>18</v>
       </c>
       <c r="G5">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="H5">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="I5">
-        <v>75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -21287,28 +21287,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -21316,31 +21316,31 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -21348,28 +21348,28 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>106</v>
+        <v>59</v>
       </c>
       <c r="C8">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="D8">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="E8">
+        <v>65</v>
+      </c>
+      <c r="F8">
+        <v>51</v>
+      </c>
+      <c r="G8">
+        <v>49</v>
+      </c>
+      <c r="H8">
+        <v>73</v>
+      </c>
+      <c r="I8">
         <v>121</v>
-      </c>
-      <c r="F8">
-        <v>146</v>
-      </c>
-      <c r="G8">
-        <v>136</v>
-      </c>
-      <c r="H8">
-        <v>180</v>
-      </c>
-      <c r="I8">
-        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -21377,28 +21377,28 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>179</v>
+        <v>67</v>
       </c>
       <c r="D9">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="E9">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="F9">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="G9">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="H9">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="I9">
-        <v>108</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -21406,28 +21406,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>478</v>
+        <v>270</v>
       </c>
       <c r="C10">
-        <v>529</v>
+        <v>365</v>
       </c>
       <c r="D10">
-        <v>455</v>
+        <v>374</v>
       </c>
       <c r="E10">
-        <v>496</v>
+        <v>354</v>
       </c>
       <c r="F10">
-        <v>432</v>
+        <v>344</v>
       </c>
       <c r="G10">
-        <v>376</v>
+        <v>236</v>
       </c>
       <c r="H10">
-        <v>325</v>
+        <v>240</v>
       </c>
       <c r="I10">
-        <v>396</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -21435,31 +21435,31 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1101</v>
+        <v>447</v>
       </c>
       <c r="C11">
-        <v>1261</v>
+        <v>564</v>
       </c>
       <c r="D11">
-        <v>1201</v>
+        <v>577</v>
       </c>
       <c r="E11">
-        <v>1159</v>
+        <v>570</v>
       </c>
       <c r="F11">
-        <v>1120</v>
+        <v>531</v>
       </c>
       <c r="G11">
-        <v>1064</v>
+        <v>422</v>
       </c>
       <c r="H11">
-        <v>1027</v>
+        <v>454</v>
       </c>
       <c r="I11">
-        <v>1103</v>
+        <v>581</v>
       </c>
       <c r="J11">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -35166,7 +35166,7 @@
 
 <file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35216,181 +35216,230 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
       <c r="I2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3">
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="I5">
         <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
       <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H8">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>86</v>
+      </c>
+      <c r="C10">
+        <v>113</v>
+      </c>
+      <c r="D10">
+        <v>116</v>
+      </c>
+      <c r="E10">
+        <v>102</v>
+      </c>
+      <c r="F10">
+        <v>128</v>
+      </c>
+      <c r="G10">
+        <v>49</v>
+      </c>
+      <c r="H10">
+        <v>77</v>
+      </c>
+      <c r="I10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>43</v>
-      </c>
-      <c r="C9">
-        <v>49</v>
-      </c>
-      <c r="D9">
-        <v>76</v>
-      </c>
-      <c r="E9">
-        <v>73</v>
-      </c>
-      <c r="F9">
-        <v>48</v>
-      </c>
-      <c r="G9">
-        <v>37</v>
-      </c>
-      <c r="H9">
-        <v>18</v>
-      </c>
-      <c r="I9">
-        <v>56</v>
+      <c r="B11">
+        <v>95</v>
+      </c>
+      <c r="C11">
+        <v>128</v>
+      </c>
+      <c r="D11">
+        <v>149</v>
+      </c>
+      <c r="E11">
+        <v>124</v>
+      </c>
+      <c r="F11">
+        <v>154</v>
+      </c>
+      <c r="G11">
+        <v>79</v>
+      </c>
+      <c r="H11">
+        <v>95</v>
+      </c>
+      <c r="I11">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -35690,7 +35739,7 @@
 
 <file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35740,230 +35789,181 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>3</v>
+      <c r="C3">
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
       <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I8">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D9">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>48</v>
+      </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9">
         <v>18</v>
       </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>6</v>
-      </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
       <c r="I9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>86</v>
-      </c>
-      <c r="C10">
-        <v>113</v>
-      </c>
-      <c r="D10">
-        <v>116</v>
-      </c>
-      <c r="E10">
-        <v>102</v>
-      </c>
-      <c r="F10">
-        <v>128</v>
-      </c>
-      <c r="G10">
-        <v>49</v>
-      </c>
-      <c r="H10">
-        <v>77</v>
-      </c>
-      <c r="I10">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>95</v>
-      </c>
-      <c r="C11">
-        <v>128</v>
-      </c>
-      <c r="D11">
-        <v>149</v>
-      </c>
-      <c r="E11">
-        <v>124</v>
-      </c>
-      <c r="F11">
-        <v>154</v>
-      </c>
-      <c r="G11">
-        <v>79</v>
-      </c>
-      <c r="H11">
-        <v>95</v>
-      </c>
-      <c r="I11">
-        <v>187</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add data for 2023-07-28
</commit_message>
<xml_diff>
--- a/output/index-crime-ytd.xlsx
+++ b/output/index-crime-ytd.xlsx
@@ -102,9 +102,9 @@
     <sheet name="Burnside" sheetId="93" r:id="rId93"/>
     <sheet name="Sauganash,Forest Glen" sheetId="94" r:id="rId94"/>
     <sheet name="Rush &amp; Division" sheetId="95" r:id="rId95"/>
-    <sheet name="Printers Row" sheetId="96" r:id="rId96"/>
+    <sheet name="Grant Park" sheetId="96" r:id="rId96"/>
     <sheet name="Gold Coast" sheetId="97" r:id="rId97"/>
-    <sheet name="Grant Park" sheetId="98" r:id="rId98"/>
+    <sheet name="Printers Row" sheetId="98" r:id="rId98"/>
     <sheet name="Museum Campus" sheetId="99" r:id="rId99"/>
     <sheet name="Millenium Park" sheetId="100" r:id="rId100"/>
   </sheets>
@@ -35375,7 +35375,7 @@
 
 <file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35425,236 +35425,184 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>1</v>
-      </c>
-      <c r="G5">
-        <v>11</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="G8">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I8">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D9">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="F9">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>109</v>
-      </c>
-      <c r="C10">
-        <v>124</v>
-      </c>
-      <c r="D10">
-        <v>127</v>
-      </c>
-      <c r="E10">
-        <v>118</v>
-      </c>
-      <c r="F10">
-        <v>141</v>
-      </c>
-      <c r="G10">
-        <v>55</v>
-      </c>
-      <c r="H10">
-        <v>91</v>
-      </c>
-      <c r="I10">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>120</v>
-      </c>
-      <c r="C11">
-        <v>141</v>
-      </c>
-      <c r="D11">
-        <v>163</v>
-      </c>
-      <c r="E11">
-        <v>144</v>
-      </c>
-      <c r="F11">
-        <v>169</v>
-      </c>
-      <c r="G11">
-        <v>88</v>
-      </c>
-      <c r="H11">
-        <v>112</v>
-      </c>
-      <c r="I11">
-        <v>213</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -35954,7 +35902,7 @@
 
 <file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36004,184 +35952,236 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="I5">
         <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="H8">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I8">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>56</v>
-      </c>
-      <c r="C9">
-        <v>65</v>
-      </c>
-      <c r="D9">
-        <v>84</v>
-      </c>
-      <c r="E9">
-        <v>83</v>
-      </c>
       <c r="F9">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="I9">
-        <v>76</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>109</v>
+      </c>
+      <c r="C10">
+        <v>124</v>
+      </c>
+      <c r="D10">
+        <v>127</v>
+      </c>
+      <c r="E10">
+        <v>118</v>
+      </c>
+      <c r="F10">
+        <v>141</v>
+      </c>
+      <c r="G10">
+        <v>55</v>
+      </c>
+      <c r="H10">
+        <v>91</v>
+      </c>
+      <c r="I10">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <v>141</v>
+      </c>
+      <c r="D11">
+        <v>163</v>
+      </c>
+      <c r="E11">
+        <v>144</v>
+      </c>
+      <c r="F11">
+        <v>169</v>
+      </c>
+      <c r="G11">
+        <v>88</v>
+      </c>
+      <c r="H11">
+        <v>112</v>
+      </c>
+      <c r="I11">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>